<commit_message>
Adding variable "strata" in the data
Adding an entire column in the data, that is "strata
</commit_message>
<xml_diff>
--- a/input/sample/Final_sampling_summary_WB_Gaza_EJ.xlsx
+++ b/input/sample/Final_sampling_summary_WB_Gaza_EJ.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael BALLY\Documents\REACH2021\2. Coordination\3. PCBS\Research_Design_PCBS_03062021\1. Sampling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evelyn GAKINYA\Documents\2. Data cleaning\MSNA_Data_Cleaning_Opt\input\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14480" windowHeight="5150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14484" windowHeight="5148" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="West Bank" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="111">
   <si>
     <t>Stratification</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Nablus_C</t>
   </si>
   <si>
-    <t>Qalqilya_C</t>
-  </si>
-  <si>
     <t>Ramallah_C</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Tubas_C</t>
   </si>
   <si>
-    <t>Tulkarem_C</t>
-  </si>
-  <si>
     <t>WB_Camps</t>
   </si>
   <si>
@@ -210,6 +204,156 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>area_AB</t>
+  </si>
+  <si>
+    <t>bethlehem_C</t>
+  </si>
+  <si>
+    <t>hebron_C</t>
+  </si>
+  <si>
+    <t>jenin_C</t>
+  </si>
+  <si>
+    <t>jericho_C</t>
+  </si>
+  <si>
+    <t>nablus_C</t>
+  </si>
+  <si>
+    <t>ramallah_C</t>
+  </si>
+  <si>
+    <t>salfit_C</t>
+  </si>
+  <si>
+    <t>tubas_C</t>
+  </si>
+  <si>
+    <t>wb_Camps</t>
+  </si>
+  <si>
+    <t>jerusalem_2_C</t>
+  </si>
+  <si>
+    <t>qalqiliya_C</t>
+  </si>
+  <si>
+    <t>Qalqiliya_C</t>
+  </si>
+  <si>
+    <t>Tulkarm_C</t>
+  </si>
+  <si>
+    <t>tulkarm_C</t>
+  </si>
+  <si>
+    <t>umm_naser</t>
+  </si>
+  <si>
+    <t>beit_hanun</t>
+  </si>
+  <si>
+    <t>beit_lahiya</t>
+  </si>
+  <si>
+    <t>jabalya_camp</t>
+  </si>
+  <si>
+    <t>jabalya</t>
+  </si>
+  <si>
+    <t>shati_camp</t>
+  </si>
+  <si>
+    <t>gaza</t>
+  </si>
+  <si>
+    <t>madinat_ezahra</t>
+  </si>
+  <si>
+    <t>al_mughraqa</t>
+  </si>
+  <si>
+    <t>juhor_ad_dik</t>
+  </si>
+  <si>
+    <t>nuseirat_camp</t>
+  </si>
+  <si>
+    <t>an_nuseirat</t>
+  </si>
+  <si>
+    <t>bureij_camp</t>
+  </si>
+  <si>
+    <t>al_bureij</t>
+  </si>
+  <si>
+    <t>az_zawayda</t>
+  </si>
+  <si>
+    <t>deir_balah_camp</t>
+  </si>
+  <si>
+    <t>maghazi_camp</t>
+  </si>
+  <si>
+    <t>al_maghazi</t>
+  </si>
+  <si>
+    <t>deir_balah</t>
+  </si>
+  <si>
+    <t>al_musaddar</t>
+  </si>
+  <si>
+    <t>wadi_salqa</t>
+  </si>
+  <si>
+    <t>al_qarara</t>
+  </si>
+  <si>
+    <t>khan_yunis_camp</t>
+  </si>
+  <si>
+    <t>khan_yunis</t>
+  </si>
+  <si>
+    <t>bani_suheila</t>
+  </si>
+  <si>
+    <t>abasan_jadida</t>
+  </si>
+  <si>
+    <t>abasan_kabira</t>
+  </si>
+  <si>
+    <t>khuza</t>
+  </si>
+  <si>
+    <t>al_fukhari</t>
+  </si>
+  <si>
+    <t>rafah</t>
+  </si>
+  <si>
+    <t>rafah_camp</t>
+  </si>
+  <si>
+    <t>an_naser</t>
+  </si>
+  <si>
+    <t>ash_shoka</t>
+  </si>
+  <si>
+    <t>strata</t>
+  </si>
+  <si>
+    <t>East_Jerusalem</t>
   </si>
 </sst>
 </file>
@@ -1046,673 +1190,714 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2">
         <v>200</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>25</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
       </c>
       <c r="F2">
         <v>8</v>
       </c>
       <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
         <v>0.06</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.42</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>141</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.15</v>
       </c>
-      <c r="K2">
-        <v>0.95</v>
-      </c>
       <c r="L2">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M2">
+        <v>0.09</v>
+      </c>
+      <c r="N2">
         <v>465190</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3">
         <v>208</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>21</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>9.9</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.06</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1.534</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>136</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.15</v>
       </c>
-      <c r="K3">
-        <v>0.95</v>
-      </c>
       <c r="L3">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M3">
+        <v>0.09</v>
+      </c>
+      <c r="N3">
         <v>6157</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
         <v>216</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>21</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>10.29</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.06</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.5573999999999999</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>139</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.15</v>
       </c>
-      <c r="K4">
-        <v>0.95</v>
-      </c>
       <c r="L4">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M4">
+        <v>0.09</v>
+      </c>
+      <c r="N4">
         <v>7712</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5">
         <v>200</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>24</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8.33</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.06</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1.4398</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>139</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.15</v>
       </c>
-      <c r="K5">
-        <v>0.95</v>
-      </c>
       <c r="L5">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M5">
+        <v>0.09</v>
+      </c>
+      <c r="N5">
         <v>12089</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
         <v>208</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>22</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>9.4499999999999993</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>8</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.06</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1.5069999999999999</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>138</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.15</v>
       </c>
-      <c r="K6">
-        <v>0.95</v>
-      </c>
       <c r="L6">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M6">
+        <v>0.09</v>
+      </c>
+      <c r="N6">
         <v>4122</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7">
         <v>240</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>16</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>8</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.06</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.9</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>126</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.15</v>
       </c>
-      <c r="K7">
-        <v>0.95</v>
-      </c>
       <c r="L7">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M7">
+        <v>0.09</v>
+      </c>
+      <c r="N7">
         <v>1120</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8">
         <v>208</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>21</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>9.9</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>8</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.06</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1.534</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>136</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.15</v>
       </c>
-      <c r="K8">
-        <v>0.95</v>
-      </c>
       <c r="L8">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M8">
+        <v>0.09</v>
+      </c>
+      <c r="N8">
         <v>7583</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
         <v>216</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>19</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>11.37</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.06</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1.6222000000000001</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>133</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.15</v>
       </c>
-      <c r="K9">
-        <v>0.95</v>
-      </c>
       <c r="L9">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M9">
+        <v>0.09</v>
+      </c>
+      <c r="N9">
         <v>2403</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10">
         <v>216</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>10.8</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>8</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.06</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1.5880000000000001</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>136</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.15</v>
       </c>
-      <c r="K10">
-        <v>0.95</v>
-      </c>
       <c r="L10">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M10">
+        <v>0.09</v>
+      </c>
+      <c r="N10">
         <v>2593</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11">
         <v>208</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>21</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>9.9</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.06</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1.534</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>136</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.15</v>
       </c>
-      <c r="K11">
-        <v>0.95</v>
-      </c>
       <c r="L11">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M11">
+        <v>0.09</v>
+      </c>
+      <c r="N11">
         <v>5431</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12">
         <v>224</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>18</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>12.44</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>8</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.06</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1.6863999999999999</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>133</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.15</v>
       </c>
-      <c r="K12">
-        <v>0.95</v>
-      </c>
       <c r="L12">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M12">
+        <v>0.09</v>
+      </c>
+      <c r="N12">
         <v>1872</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
         <v>216</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>11</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>19.64</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>8</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.06</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2.1183999999999998</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>102</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.15</v>
       </c>
-      <c r="K13">
-        <v>0.95</v>
-      </c>
       <c r="L13">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M13">
+        <v>0.09</v>
+      </c>
+      <c r="N13">
         <v>335</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14">
         <v>216</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>19</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>11.37</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>8</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.06</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>1.6222000000000001</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>133</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.15</v>
       </c>
-      <c r="K14">
-        <v>0.95</v>
-      </c>
       <c r="L14">
-        <v>0.09</v>
+        <v>0.95</v>
       </c>
       <c r="M14">
+        <v>0.09</v>
+      </c>
+      <c r="N14">
         <v>3500</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
         <v>555</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>87</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>6.38</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>5</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.06</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1.3228</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>420</v>
       </c>
-      <c r="J15">
-        <v>0.1</v>
-      </c>
       <c r="K15">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="L15">
+        <v>0.95</v>
+      </c>
+      <c r="M15">
         <v>0.05</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>20859</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C16">
-        <f>SUM(C2:C15)</f>
-        <v>3331</v>
       </c>
     </row>
   </sheetData>
@@ -1722,1105 +1907,1206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="2">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="2">
         <v>116.60000000000001</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
         <v>106</v>
       </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
       <c r="G2">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H2">
-        <v>0.09</v>
-      </c>
-      <c r="I2" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I2">
+        <v>0.09</v>
+      </c>
+      <c r="J2" s="2">
         <v>939.00131829283214</v>
       </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="2">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="2">
         <v>129.80000000000001</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
         <v>118</v>
       </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
       <c r="G3">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
-        <v>0.09</v>
-      </c>
-      <c r="I3" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I3">
+        <v>0.09</v>
+      </c>
+      <c r="J3" s="2">
         <v>17808.317591891802</v>
       </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="2">
         <v>129.80000000000001</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>118</v>
       </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
       <c r="G4">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H4">
-        <v>0.09</v>
-      </c>
-      <c r="I4" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I4">
+        <v>0.09</v>
+      </c>
+      <c r="J4" s="2">
         <v>10354.784011750617</v>
       </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="2">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="2">
         <v>129.80000000000001</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
         <v>118</v>
       </c>
-      <c r="F5">
-        <v>0.1</v>
-      </c>
       <c r="G5">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H5">
-        <v>0.09</v>
-      </c>
-      <c r="I5" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I5">
+        <v>0.09</v>
+      </c>
+      <c r="J5" s="2">
         <v>9804.7040754486097</v>
       </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2">
         <v>130.9</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
         <v>119</v>
       </c>
-      <c r="F6">
-        <v>0.1</v>
-      </c>
       <c r="G6">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H6">
-        <v>0.09</v>
-      </c>
-      <c r="I6" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I6">
+        <v>0.09</v>
+      </c>
+      <c r="J6" s="2">
         <v>34234.596511388067</v>
       </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>117</v>
       </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
       <c r="G7">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H7">
-        <v>0.09</v>
-      </c>
-      <c r="I7" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I7">
+        <v>0.09</v>
+      </c>
+      <c r="J7" s="2">
         <v>7813.1075686832755</v>
       </c>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="2">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="2">
         <v>130.9</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
         <v>119</v>
       </c>
-      <c r="F8">
-        <v>0.1</v>
-      </c>
       <c r="G8">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H8">
-        <v>0.09</v>
-      </c>
-      <c r="I8" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I8">
+        <v>0.09</v>
+      </c>
+      <c r="J8" s="2">
         <v>113258.98684793217</v>
       </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="2">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="2">
         <v>117.7</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
         <v>107</v>
       </c>
-      <c r="F9">
-        <v>0.1</v>
-      </c>
       <c r="G9">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H9">
-        <v>0.09</v>
-      </c>
-      <c r="I9" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I9">
+        <v>0.09</v>
+      </c>
+      <c r="J9" s="2">
         <v>1023.8711690880182</v>
       </c>
-      <c r="J9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="2">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="2">
         <v>124.30000000000001</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <v>113</v>
       </c>
-      <c r="F10">
-        <v>0.1</v>
-      </c>
       <c r="G10">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H10">
-        <v>0.09</v>
-      </c>
-      <c r="I10" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I10">
+        <v>0.09</v>
+      </c>
+      <c r="J10" s="2">
         <v>2197.7362037112234</v>
       </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="2">
         <v>115.50000000000001</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
         <v>105</v>
       </c>
-      <c r="F11">
-        <v>0.1</v>
-      </c>
       <c r="G11">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H11">
-        <v>0.09</v>
-      </c>
-      <c r="I11" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I11">
+        <v>0.09</v>
+      </c>
+      <c r="J11" s="2">
         <v>879.63154391863077</v>
       </c>
-      <c r="J11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="2">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
         <v>117</v>
       </c>
-      <c r="F12">
-        <v>0.1</v>
-      </c>
       <c r="G12">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H12">
-        <v>0.09</v>
-      </c>
-      <c r="I12" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I12">
+        <v>0.09</v>
+      </c>
+      <c r="J12" s="2">
         <v>6391.3814248635699</v>
       </c>
-      <c r="J12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="2">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="2">
         <v>129.80000000000001</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
         <v>118</v>
       </c>
-      <c r="F13">
-        <v>0.1</v>
-      </c>
       <c r="G13">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H13">
-        <v>0.09</v>
-      </c>
-      <c r="I13" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I13">
+        <v>0.09</v>
+      </c>
+      <c r="J13" s="2">
         <v>11042.733566484761</v>
       </c>
-      <c r="J13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="2">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
         <v>117</v>
       </c>
-      <c r="F14">
-        <v>0.1</v>
-      </c>
       <c r="G14">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H14">
-        <v>0.09</v>
-      </c>
-      <c r="I14" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I14">
+        <v>0.09</v>
+      </c>
+      <c r="J14" s="2">
         <v>5641.8582244110212</v>
       </c>
-      <c r="J14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="2">
         <v>126.50000000000001</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <v>115</v>
       </c>
-      <c r="F15">
-        <v>0.1</v>
-      </c>
       <c r="G15">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H15">
-        <v>0.09</v>
-      </c>
-      <c r="I15" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I15">
+        <v>0.09</v>
+      </c>
+      <c r="J15" s="2">
         <v>3118.6849041661121</v>
       </c>
-      <c r="J15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="2">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="2">
         <v>127.60000000000001</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
         <v>116</v>
       </c>
-      <c r="F16">
-        <v>0.1</v>
-      </c>
       <c r="G16">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H16">
-        <v>0.09</v>
-      </c>
-      <c r="I16" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I16">
+        <v>0.09</v>
+      </c>
+      <c r="J16" s="2">
         <v>4799.7267316651141</v>
       </c>
-      <c r="J16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="2">
         <v>121.00000000000001</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
         <v>110</v>
       </c>
-      <c r="F17">
-        <v>0.1</v>
-      </c>
       <c r="G17">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H17">
-        <v>0.09</v>
-      </c>
-      <c r="I17" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I17">
+        <v>0.09</v>
+      </c>
+      <c r="J17" s="2">
         <v>1406.2367862371889</v>
       </c>
-      <c r="J17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="2">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="2">
         <v>126.50000000000001</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
         <v>115</v>
       </c>
-      <c r="F18">
-        <v>0.1</v>
-      </c>
       <c r="G18">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H18">
-        <v>0.09</v>
-      </c>
-      <c r="I18" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I18">
+        <v>0.09</v>
+      </c>
+      <c r="J18" s="2">
         <v>3655.4103547184886</v>
       </c>
-      <c r="J18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="2">
         <v>123.20000000000002</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
         <v>112</v>
       </c>
-      <c r="F19">
-        <v>0.1</v>
-      </c>
       <c r="G19">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H19">
-        <v>0.09</v>
-      </c>
-      <c r="I19" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I19">
+        <v>0.09</v>
+      </c>
+      <c r="J19" s="2">
         <v>1946.7873619060294</v>
       </c>
-      <c r="J19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="2">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2">
         <v>129.80000000000001</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>118</v>
       </c>
-      <c r="F20">
-        <v>0.1</v>
-      </c>
       <c r="G20">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H20">
-        <v>0.09</v>
-      </c>
-      <c r="I20" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I20">
+        <v>0.09</v>
+      </c>
+      <c r="J20" s="2">
         <v>15125.752644749102</v>
       </c>
-      <c r="J20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="2">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="2">
         <v>106.7</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
         <v>97</v>
       </c>
-      <c r="F21">
-        <v>0.1</v>
-      </c>
       <c r="G21">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H21">
-        <v>0.09</v>
-      </c>
-      <c r="I21" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I21">
+        <v>0.09</v>
+      </c>
+      <c r="J21" s="2">
         <v>520.82098296286426</v>
       </c>
-      <c r="J21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="2">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="2">
         <v>121.00000000000001</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
         <v>110</v>
       </c>
-      <c r="F22">
-        <v>0.1</v>
-      </c>
       <c r="G22">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H22">
-        <v>0.09</v>
-      </c>
-      <c r="I22" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I22">
+        <v>0.09</v>
+      </c>
+      <c r="J22" s="2">
         <v>1351.8797451084788</v>
       </c>
-      <c r="J22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
         <v>117</v>
       </c>
-      <c r="F23">
-        <v>0.1</v>
-      </c>
       <c r="G23">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H23">
-        <v>0.09</v>
-      </c>
-      <c r="I23" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I23">
+        <v>0.09</v>
+      </c>
+      <c r="J23" s="2">
         <v>5886.5268232811331</v>
       </c>
-      <c r="J23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="2">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
         <v>117</v>
       </c>
-      <c r="F24">
-        <v>0.1</v>
-      </c>
       <c r="G24">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H24">
-        <v>0.09</v>
-      </c>
-      <c r="I24" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I24">
+        <v>0.09</v>
+      </c>
+      <c r="J24" s="2">
         <v>8358.121212121212</v>
       </c>
-      <c r="J24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="2">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="2">
         <v>130.9</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
         <v>119</v>
       </c>
-      <c r="F25">
-        <v>0.1</v>
-      </c>
       <c r="G25">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H25">
-        <v>0.09</v>
-      </c>
-      <c r="I25" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I25">
+        <v>0.09</v>
+      </c>
+      <c r="J25" s="2">
         <v>41631.285844212616</v>
       </c>
-      <c r="J25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="2">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
         <v>117</v>
       </c>
-      <c r="F26">
-        <v>0.1</v>
-      </c>
       <c r="G26">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H26">
-        <v>0.09</v>
-      </c>
-      <c r="I26" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I26">
+        <v>0.09</v>
+      </c>
+      <c r="J26" s="2">
         <v>8410.2808243672207</v>
       </c>
-      <c r="J26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="2">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="2">
         <v>123.20000000000002</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
         <v>112</v>
       </c>
-      <c r="F27">
-        <v>0.1</v>
-      </c>
       <c r="G27">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H27">
-        <v>0.09</v>
-      </c>
-      <c r="I27" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I27">
+        <v>0.09</v>
+      </c>
+      <c r="J27" s="2">
         <v>1885.4583570639129</v>
       </c>
-      <c r="J27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
         <v>117</v>
       </c>
-      <c r="F28">
-        <v>0.1</v>
-      </c>
       <c r="G28">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H28">
-        <v>0.09</v>
-      </c>
-      <c r="I28" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I28">
+        <v>0.09</v>
+      </c>
+      <c r="J28" s="2">
         <v>5432.5149454822122</v>
       </c>
-      <c r="J28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="2">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="2">
         <v>124.30000000000001</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
         <v>113</v>
       </c>
-      <c r="F29">
-        <v>0.1</v>
-      </c>
       <c r="G29">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H29">
-        <v>0.09</v>
-      </c>
-      <c r="I29" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I29">
+        <v>0.09</v>
+      </c>
+      <c r="J29" s="2">
         <v>2311.2593939982607</v>
       </c>
-      <c r="J29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="2">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="2">
         <v>119.9</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
         <v>109</v>
       </c>
-      <c r="F30">
-        <v>0.1</v>
-      </c>
       <c r="G30">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H30">
-        <v>0.09</v>
-      </c>
-      <c r="I30" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I30">
+        <v>0.09</v>
+      </c>
+      <c r="J30" s="2">
         <v>1307.6435085643477</v>
       </c>
-      <c r="J30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="2">
         <v>130.9</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
         <v>119</v>
       </c>
-      <c r="F31">
-        <v>0.1</v>
-      </c>
       <c r="G31">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H31">
-        <v>0.09</v>
-      </c>
-      <c r="I31" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I31">
+        <v>0.09</v>
+      </c>
+      <c r="J31" s="2">
         <v>34140.092104644304</v>
       </c>
-      <c r="J31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="2">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="2">
         <v>128.70000000000002</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
         <v>117</v>
       </c>
-      <c r="F32">
-        <v>0.1</v>
-      </c>
       <c r="G32">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H32">
-        <v>0.09</v>
-      </c>
-      <c r="I32" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I32">
+        <v>0.09</v>
+      </c>
+      <c r="J32" s="2">
         <v>7259.0321434374209</v>
       </c>
-      <c r="J32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="2">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="2">
         <v>123.20000000000002</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
         <v>112</v>
       </c>
-      <c r="F33">
-        <v>0.1</v>
-      </c>
       <c r="G33">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H33">
-        <v>0.09</v>
-      </c>
-      <c r="I33" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I33">
+        <v>0.09</v>
+      </c>
+      <c r="J33" s="2">
         <v>1784.272086912224</v>
       </c>
-      <c r="J33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="2">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="2">
         <v>126.50000000000001</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3">
         <v>115</v>
       </c>
-      <c r="F34">
-        <v>0.1</v>
-      </c>
       <c r="G34">
-        <v>0.95</v>
+        <v>0.1</v>
       </c>
       <c r="H34">
-        <v>0.09</v>
-      </c>
-      <c r="I34" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="I34">
+        <v>0.09</v>
+      </c>
+      <c r="J34" s="2">
         <v>3266.067950720339</v>
       </c>
-      <c r="J34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C35" s="1">
-        <f>SUM(C2:C34)</f>
-        <v>4145.8999999999996</v>
-      </c>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2829,16 +3115,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.26953125" customWidth="1"/>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2878,13 +3166,16 @@
       <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2">
         <v>175</v>
@@ -2922,11 +3213,12 @@
       <c r="N2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C3" s="4">
-        <v>175</v>
-      </c>
+      <c r="O2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>